<commit_message>
More POX code tweaks, so close
</commit_message>
<xml_diff>
--- a/hdw/Pulse_Oximeter/Pulse_Oximeter_BOM.xlsx
+++ b/hdw/Pulse_Oximeter/Pulse_Oximeter_BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\pulse_oximeter\hdw\Pulse_Oximeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2122849C-D889-456B-8833-D4D93A5809F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3785DD8-34F9-4FBE-B5FC-8B406D316486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020"/>
+    <workbookView xWindow="38280" yWindow="3540" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pulse_Oximeter_BOM" sheetId="1" r:id="rId1"/>
@@ -580,8 +580,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,6 +712,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1058,9 +1065,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1417,11 +1427,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1452,7 +1462,7 @@
       <c r="A2" s="1">
         <v>51</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1467,7 +1477,7 @@
       <c r="A3" s="1">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>164</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1482,7 +1492,7 @@
       <c r="A4" s="1">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1512,7 +1522,7 @@
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1527,7 +1537,7 @@
       <c r="A7" s="1">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1542,7 +1552,7 @@
       <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1557,7 +1567,7 @@
       <c r="A9" s="1">
         <v>1</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1572,7 +1582,7 @@
       <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>167</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1587,7 +1597,7 @@
       <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1602,7 +1612,7 @@
       <c r="A12" s="1">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1617,7 +1627,7 @@
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1632,7 +1642,7 @@
       <c r="A14" s="1">
         <v>5</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1647,7 +1657,7 @@
       <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1731,7 +1741,7 @@
       <c r="A21" s="1">
         <v>1</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1746,7 +1756,7 @@
       <c r="A22" s="1">
         <v>5</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1791,7 +1801,7 @@
       <c r="A25" s="1">
         <v>1</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1806,7 +1816,7 @@
       <c r="A26" s="1">
         <v>2</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>174</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1821,7 +1831,7 @@
       <c r="A27" s="1">
         <v>1</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1836,7 +1846,7 @@
       <c r="A28" s="1">
         <v>1</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1851,7 +1861,7 @@
       <c r="A29" s="1">
         <v>1</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1866,7 +1876,7 @@
       <c r="A30" s="1">
         <v>2</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>175</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1881,7 +1891,7 @@
       <c r="A31" s="1">
         <v>1</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1896,7 +1906,7 @@
       <c r="A32" s="1">
         <v>2</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1911,7 +1921,7 @@
       <c r="A33" s="1">
         <v>4</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>177</v>
       </c>
       <c r="C33" s="1">
@@ -1926,7 +1936,7 @@
       <c r="A34" s="1">
         <v>39</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>178</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1941,7 +1951,7 @@
       <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1956,7 +1966,7 @@
       <c r="A36" s="1">
         <v>1</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1971,7 +1981,7 @@
       <c r="A37" s="1">
         <v>1</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1986,7 +1996,7 @@
       <c r="A38" s="1">
         <v>1</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -2001,7 +2011,7 @@
       <c r="A39" s="1">
         <v>10</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>179</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -2016,7 +2026,7 @@
       <c r="A40" s="1">
         <v>1</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C40" s="1">
@@ -2031,7 +2041,7 @@
       <c r="A41" s="1">
         <v>1</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -2046,7 +2056,7 @@
       <c r="A42" s="1">
         <v>1</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>101</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -2061,7 +2071,7 @@
       <c r="A43" s="1">
         <v>1</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -2076,7 +2086,7 @@
       <c r="A44" s="1">
         <v>2</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C44" s="1">
@@ -2091,7 +2101,7 @@
       <c r="A45" s="1">
         <v>2</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>181</v>
       </c>
       <c r="C45" s="1">
@@ -2147,7 +2157,7 @@
       <c r="A49" s="1">
         <v>1</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>115</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -2162,7 +2172,7 @@
       <c r="A50" s="1">
         <v>1</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -2177,7 +2187,7 @@
       <c r="A51" s="1">
         <v>1</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -2192,7 +2202,7 @@
       <c r="A52" s="1">
         <v>1</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -2207,7 +2217,7 @@
       <c r="A53" s="1">
         <v>1</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -2222,7 +2232,7 @@
       <c r="A54" s="1">
         <v>1</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -2237,7 +2247,7 @@
       <c r="A55" s="1">
         <v>1</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="2" t="s">
         <v>133</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -2252,7 +2262,7 @@
       <c r="A56" s="1">
         <v>1</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>136</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -2267,7 +2277,7 @@
       <c r="A57" s="1">
         <v>1</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="2" t="s">
         <v>139</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -2282,7 +2292,7 @@
       <c r="A58" s="1">
         <v>1</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="2" t="s">
         <v>142</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -2297,7 +2307,7 @@
       <c r="A59" s="1">
         <v>1</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="2" t="s">
         <v>145</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -2312,7 +2322,7 @@
       <c r="A60" s="1">
         <v>2</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="2" t="s">
         <v>182</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -2342,7 +2352,7 @@
       <c r="A62" s="1">
         <v>2</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="2" t="s">
         <v>183</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -2357,7 +2367,7 @@
       <c r="A63" s="1">
         <v>1</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>155</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -2372,7 +2382,7 @@
       <c r="A64" s="1">
         <v>8</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -2387,7 +2397,7 @@
       <c r="A65" s="1">
         <v>1</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="2" t="s">
         <v>160</v>
       </c>
       <c r="C65" s="1" t="s">

</xml_diff>